<commit_message>
Added new game UI elements. Fixed stars rendering on top of UI
</commit_message>
<xml_diff>
--- a/goods.xlsx
+++ b/goods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peric\Documents\GitHub\Trade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B294567C-450D-40F0-8025-2C10ACC83C2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081D12F5-5FAE-4C22-A884-B02460C212E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="890" yWindow="1770" windowWidth="16590" windowHeight="15460" xr2:uid="{05C397A0-17A8-4E9D-B19A-A5E239D9B74D}"/>
+    <workbookView xWindow="8020" yWindow="5190" windowWidth="16590" windowHeight="15460" xr2:uid="{05C397A0-17A8-4E9D-B19A-A5E239D9B74D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -54,9 +54,6 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Dependencies</t>
-  </si>
-  <si>
     <t>Category</t>
   </si>
   <si>
@@ -196,6 +193,9 @@
   </si>
   <si>
     <t>Pants</t>
+  </si>
+  <si>
+    <t>Components</t>
   </si>
 </sst>
 </file>
@@ -281,7 +281,7 @@
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{D87C9CCA-5192-4F43-9723-40D4A17712BC}" uniqueName="1" name="Index" queryTableFieldId="1"/>
     <tableColumn id="2" xr3:uid="{2707F75C-4314-4D65-BBE4-9E5C74D84D04}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{7763CC80-F753-4B99-A515-4E00CD7A76BD}" uniqueName="3" name="Dependencies" queryTableFieldId="3" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{7763CC80-F753-4B99-A515-4E00CD7A76BD}" uniqueName="3" name="Components" queryTableFieldId="3" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{23C6E4A7-D823-47BB-BDDE-5E6ED9D6C998}" uniqueName="4" name="Category" queryTableFieldId="4" dataDxfId="0"/>
     <tableColumn id="5" xr3:uid="{CD3D68D3-EFCF-4C5B-A5C8-608198CFE05D}" uniqueName="5" name="Found" queryTableFieldId="5"/>
   </tableColumns>
@@ -588,7 +588,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9060516-8C63-49E8-98D9-C0FC2BD34607}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
@@ -607,13 +609,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -621,13 +623,13 @@
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E2">
         <v>2</v>
@@ -638,13 +640,13 @@
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E3">
         <v>3</v>
@@ -655,13 +657,13 @@
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E4">
         <v>99</v>
@@ -672,13 +674,13 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E5">
         <v>6</v>
@@ -689,13 +691,13 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E6">
         <v>99</v>
@@ -706,13 +708,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E7">
         <v>99</v>
@@ -723,13 +725,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>7</v>
       </c>
       <c r="E8">
         <v>345</v>
@@ -740,13 +742,13 @@
         <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="E9">
         <v>-1</v>
@@ -757,13 +759,13 @@
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
       </c>
       <c r="E10">
         <v>-1</v>
@@ -774,13 +776,13 @@
         <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>21</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
       </c>
       <c r="E11">
         <v>-1</v>
@@ -791,13 +793,13 @@
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="D12" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E12">
         <v>-1</v>
@@ -808,13 +810,13 @@
         <v>11</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>26</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>27</v>
       </c>
       <c r="E13">
         <v>-1</v>
@@ -825,13 +827,13 @@
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="D14" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="E14">
         <v>-1</v>
@@ -842,13 +844,13 @@
         <v>13</v>
       </c>
       <c r="B15" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>33</v>
       </c>
       <c r="E15">
         <v>-1</v>
@@ -859,13 +861,13 @@
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="D16" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="E16">
         <v>-1</v>
@@ -876,13 +878,13 @@
         <v>15</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="E17">
         <v>-1</v>
@@ -893,13 +895,13 @@
         <v>16</v>
       </c>
       <c r="B18" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>40</v>
-      </c>
       <c r="D18" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E18">
         <v>-1</v>
@@ -910,13 +912,13 @@
         <v>17</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>42</v>
-      </c>
       <c r="D19" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E19">
         <v>-1</v>
@@ -927,13 +929,13 @@
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="D20" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>45</v>
       </c>
       <c r="E20">
         <v>-1</v>
@@ -944,13 +946,13 @@
         <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="D21" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E21">
         <v>-1</v>
@@ -961,13 +963,13 @@
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="E22">
         <v>-1</v>

</xml_diff>

<commit_message>
Tried CSV item data, went with JSON instead and got deserialization working
</commit_message>
<xml_diff>
--- a/goods.xlsx
+++ b/goods.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peric\Documents\GitHub\Trade\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{081D12F5-5FAE-4C22-A884-B02460C212E6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E234C5CB-CE3F-4229-B1F5-A2FF1649EBCC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8020" yWindow="5190" windowWidth="16590" windowHeight="15460" xr2:uid="{05C397A0-17A8-4E9D-B19A-A5E239D9B74D}"/>
+    <workbookView xWindow="3920" yWindow="1700" windowWidth="16590" windowHeight="15460" xr2:uid="{05C397A0-17A8-4E9D-B19A-A5E239D9B74D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="51">
   <si>
     <t>Index</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Components</t>
+  </si>
+  <si>
+    <t>Mass</t>
   </si>
 </sst>
 </file>
@@ -238,7 +241,10 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
@@ -263,27 +269,29 @@
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="1" xr16:uid="{E0F1FA9B-5739-418F-93E5-96EF8D41D754}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
-  <queryTableRefresh nextId="6">
-    <queryTableFields count="5">
+  <queryTableRefresh nextId="7" unboundColumnsRight="1">
+    <queryTableFields count="6">
       <queryTableField id="1" name="Index" tableColumnId="1"/>
       <queryTableField id="2" name="Name" tableColumnId="2"/>
       <queryTableField id="3" name="Dependencies" tableColumnId="3"/>
       <queryTableField id="4" name="Category" tableColumnId="4"/>
       <queryTableField id="5" name="Found" tableColumnId="5"/>
+      <queryTableField id="6" dataBound="0" tableColumnId="6"/>
     </queryTableFields>
   </queryTableRefresh>
 </queryTable>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{007FFEFF-12BC-4B29-A91C-12697577D264}" name="goods" displayName="goods" ref="A1:E22" tableType="queryTable" totalsRowShown="0">
-  <autoFilter ref="A1:E22" xr:uid="{18307CF1-E757-464F-9307-1CCB22AE2182}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{007FFEFF-12BC-4B29-A91C-12697577D264}" name="goods" displayName="goods" ref="A1:F22" tableType="queryTable" totalsRowShown="0">
+  <autoFilter ref="A1:F22" xr:uid="{18307CF1-E757-464F-9307-1CCB22AE2182}"/>
+  <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{D87C9CCA-5192-4F43-9723-40D4A17712BC}" uniqueName="1" name="Index" queryTableFieldId="1"/>
-    <tableColumn id="2" xr3:uid="{2707F75C-4314-4D65-BBE4-9E5C74D84D04}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{7763CC80-F753-4B99-A515-4E00CD7A76BD}" uniqueName="3" name="Components" queryTableFieldId="3" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{23C6E4A7-D823-47BB-BDDE-5E6ED9D6C998}" uniqueName="4" name="Category" queryTableFieldId="4" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{2707F75C-4314-4D65-BBE4-9E5C74D84D04}" uniqueName="2" name="Name" queryTableFieldId="2" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7763CC80-F753-4B99-A515-4E00CD7A76BD}" uniqueName="3" name="Components" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="4" xr3:uid="{23C6E4A7-D823-47BB-BDDE-5E6ED9D6C998}" uniqueName="4" name="Category" queryTableFieldId="4" dataDxfId="1"/>
     <tableColumn id="5" xr3:uid="{CD3D68D3-EFCF-4C5B-A5C8-608198CFE05D}" uniqueName="5" name="Found" queryTableFieldId="5"/>
+    <tableColumn id="6" xr3:uid="{AA304693-8117-4294-83AE-E119A35BE97B}" uniqueName="6" name="Mass" queryTableFieldId="6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -586,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9060516-8C63-49E8-98D9-C0FC2BD34607}">
-  <dimension ref="A1:E22"/>
+  <dimension ref="A1:F22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -601,7 +609,7 @@
     <col min="5" max="5" width="8.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -617,8 +625,11 @@
       <c r="E1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>0</v>
       </c>
@@ -634,8 +645,11 @@
       <c r="E2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F2" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>1</v>
       </c>
@@ -651,8 +665,11 @@
       <c r="E3">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>2</v>
       </c>
@@ -668,8 +685,11 @@
       <c r="E4">
         <v>99</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>3</v>
       </c>
@@ -685,8 +705,11 @@
       <c r="E5">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F5" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>4</v>
       </c>
@@ -702,8 +725,11 @@
       <c r="E6">
         <v>99</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F6" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>5</v>
       </c>
@@ -719,8 +745,11 @@
       <c r="E7">
         <v>99</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F7" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>6</v>
       </c>
@@ -736,8 +765,11 @@
       <c r="E8">
         <v>345</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F8" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>7</v>
       </c>
@@ -753,8 +785,11 @@
       <c r="E9">
         <v>-1</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>8</v>
       </c>
@@ -770,8 +805,11 @@
       <c r="E10">
         <v>-1</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>9</v>
       </c>
@@ -787,8 +825,11 @@
       <c r="E11">
         <v>-1</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>10</v>
       </c>
@@ -804,8 +845,11 @@
       <c r="E12">
         <v>-1</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F12" s="1">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>11</v>
       </c>
@@ -821,8 +865,11 @@
       <c r="E13">
         <v>-1</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="1">
+        <v>50000000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>12</v>
       </c>
@@ -838,8 +885,11 @@
       <c r="E14">
         <v>-1</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F14" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>13</v>
       </c>
@@ -855,8 +905,11 @@
       <c r="E15">
         <v>-1</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F15" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>14</v>
       </c>
@@ -872,8 +925,11 @@
       <c r="E16">
         <v>-1</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>15</v>
       </c>
@@ -889,8 +945,11 @@
       <c r="E17">
         <v>-1</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>16</v>
       </c>
@@ -906,8 +965,11 @@
       <c r="E18">
         <v>-1</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F18" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>17</v>
       </c>
@@ -923,8 +985,11 @@
       <c r="E19">
         <v>-1</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="1">
+        <v>2500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>18</v>
       </c>
@@ -940,8 +1005,11 @@
       <c r="E20">
         <v>-1</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>19</v>
       </c>
@@ -957,8 +1025,11 @@
       <c r="E21">
         <v>-1</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="1">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>20</v>
       </c>
@@ -973,6 +1044,9 @@
       </c>
       <c r="E22">
         <v>-1</v>
+      </c>
+      <c r="F22" s="1">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>